<commit_message>
Comment out Supporting docx
</commit_message>
<xml_diff>
--- a/Data/Config/configaration file.xlsx
+++ b/Data/Config/configaration file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gulshiyaa\Documents\UiPath\Nabard-Uipath_New\Data\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C3C4826-3E72-4653-B614-AAB8E2A9BDC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB1C486-0ACF-4D6D-803F-27F794FBFB30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Case Creation" sheetId="1" r:id="rId1"/>
@@ -607,9 +607,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1198,7 +1196,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49A46176-7EC0-4001-94EF-1DDEBAB0CD43}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>